<commit_message>
Added relaxed number format option
</commit_message>
<xml_diff>
--- a/ExcelToEnumerable.Tests/TestSpreadsheets/AllNumericFormats.xlsx
+++ b/ExcelToEnumerable.Tests/TestSpreadsheets/AllNumericFormats.xlsx
@@ -135,10 +135,10 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="E:H"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>